<commit_message>
tung - commit 11
</commit_message>
<xml_diff>
--- a/uploads/AudioInfo.xlsx
+++ b/uploads/AudioInfo.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>fileName</t>
   </si>
@@ -40,13 +40,13 @@
     <t>region</t>
   </si>
   <si>
-    <t>file1402-1541520088226.wav</t>
+    <t>file1424-1542116667062.wav</t>
   </si>
   <si>
     <t>"5bdb8eaecdf71a365c6bc1cd"</t>
   </si>
   <si>
-    <t>Gà trống dậy sớm; Mèo lười ngủ trưa; Còn em đi học; Đi cho đúng giờ.</t>
+    <t>Kiến Đen uống rượu la đà; Bao nhiêu kiến Gió bay ra chia phần…</t>
   </si>
   <si>
     <t>male</t>
@@ -58,46 +58,16 @@
     <t>Thừa Thiên Huế</t>
   </si>
   <si>
-    <t>file2655-1541520088231.wav</t>
-  </si>
-  <si>
-    <t>Có nàng gà mái hoa mơ; Cục ta cục tác khi vừa đẻ xong</t>
-  </si>
-  <si>
-    <t>file3119-1541520088240.wav</t>
-  </si>
-  <si>
-    <t>Dù đi xa thật là xa; Chẳng đâu vui được như nhà của em.</t>
-  </si>
-  <si>
-    <t>file167-1541520141079.wav</t>
-  </si>
-  <si>
-    <t>Bác giun đào đất suốt ngày; Trưa nay chết dưới bóng cây sau nhà</t>
-  </si>
-  <si>
-    <t>file2232-1541520141081.wav</t>
-  </si>
-  <si>
-    <t>Kiến Lửa đốt đuốc đỏ làng; Kiến Kim chống gậy, kiến Càng nặng vai</t>
-  </si>
-  <si>
-    <t>file3185-1541520141084.wav</t>
-  </si>
-  <si>
-    <t>Đám ma đưa đến là dài; Qua những vườn chuối, vườn khoai, vườn cà</t>
-  </si>
-  <si>
-    <t>file1552-1541525696443.wav</t>
-  </si>
-  <si>
-    <t>Họ hàng nhà kiến kéo ra; Kiến con đi trước, kiến già theo sau</t>
-  </si>
-  <si>
-    <t>file2343-1541525696458.wav</t>
-  </si>
-  <si>
-    <t>file3184-1541525696469.wav</t>
+    <t>file2608-1542116667082.wav</t>
+  </si>
+  <si>
+    <t>Cầm hương kiến Đất bạc đầu; Khóc than kiến Cánh khoác màu áo tang</t>
+  </si>
+  <si>
+    <t>file3615-1542116667100.wav</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sân khấu ở trên không; Giữa vòm trời lá biếc; Trên cành những nhạc công; Cùng thổi kèn náo nhiệt </t>
   </si>
 </sst>
 </file>
@@ -474,11 +444,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="6" width="50" customWidth="1"/>
+    <col min="2" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
+    <col min="6" max="6" width="50" customWidth="1"/>
     <col min="7" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
   </cols>
@@ -517,10 +489,10 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>6741</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>48000</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -546,10 +518,10 @@
         <v>15</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>6570</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>48000</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -575,10 +547,10 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>8277</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>48000</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -596,180 +568,6 @@
         <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8">
-        <v>4096</v>
-      </c>
-      <c r="C8">
-        <v>48000</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9">
-        <v>4096</v>
-      </c>
-      <c r="C9">
-        <v>48000</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10">
-        <v>4437</v>
-      </c>
-      <c r="C10">
-        <v>48000</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>